<commit_message>
update data for new ecdc and framework
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D2E91C-77C1-5C45-BA0D-9BFFB6F3C7FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1006678E-A4BD-7B43-B5BF-F28E085B1DF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="3340" windowWidth="20720" windowHeight="16880" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>study_id</t>
   </si>
@@ -34,9 +34,6 @@
     <t>breakdown</t>
   </si>
   <si>
-    <t>ESP1</t>
-  </si>
-  <si>
     <t>ageband</t>
   </si>
   <si>
@@ -116,6 +113,21 @@
   </si>
   <si>
     <t>data/derived/USA/NYC_NY_1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/CHE/CHE_region.RDS</t>
+  </si>
+  <si>
+    <t>GBR2</t>
+  </si>
+  <si>
+    <t>data/derived/UK/GBR_regions.RDS</t>
+  </si>
+  <si>
+    <t>ESP1-2</t>
+  </si>
+  <si>
+    <t>data/derived/UK/GBR2_agebands.RDS</t>
   </si>
 </sst>
 </file>
@@ -478,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC09EBF-A19C-5D4E-8812-2D348421568B}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,183 +510,234 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -694,36 +757,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data map for Italy
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1006678E-A4BD-7B43-B5BF-F28E085B1DF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3611C58-EAD7-4492-BA2B-209524E2605A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="3340" windowWidth="20720" windowHeight="16880" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="37">
   <si>
     <t>study_id</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>data/derived/UK/GBR2_agebands.RDS</t>
+  </si>
+  <si>
+    <t>ITA1</t>
+  </si>
+  <si>
+    <t>data/derived/ITA/ITA_regions.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/ITA/ITA_agebands.RDS</t>
   </si>
 </sst>
 </file>
@@ -490,19 +499,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC09EBF-A19C-5D4E-8812-2D348421568B}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +528,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -536,7 +545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -553,7 +562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -570,7 +579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -587,7 +596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -604,7 +613,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -621,7 +630,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -638,7 +647,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -655,7 +664,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -672,7 +681,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -689,7 +698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -706,7 +715,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -723,7 +732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -738,6 +747,40 @@
       </c>
       <c r="E14" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -753,9 +796,9 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -772,7 +815,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
update bits from merge for data wrangle
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7522D3E4-EB8A-4082-B0CA-CD0F4D1149AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C252F151-E6CB-8A4E-AD2E-211FE092386C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -511,19 +511,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC09EBF-A19C-5D4E-8812-2D348421568B}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A13" sqref="A13:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="32.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -557,7 +557,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -574,7 +574,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -591,7 +591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -608,7 +608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -625,7 +625,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -642,7 +642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -659,7 +659,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -676,7 +676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -693,7 +693,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -710,7 +710,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -727,49 +727,49 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -778,54 +778,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
         <v>16</v>
       </c>
     </row>
@@ -836,15 +802,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC807514-CEE2-0E42-8077-13B94445F7E9}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -861,7 +827,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -876,6 +842,40 @@
       </c>
       <c r="E2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add GBR3 to datamap
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C252F151-E6CB-8A4E-AD2E-211FE092386C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299AFC1E-DCD6-4933-A6FD-71BF45C13998}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
   <si>
     <t>study_id</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>data/derived/UK/GBR2_regions.RDS</t>
+  </si>
+  <si>
+    <t>GBR3</t>
+  </si>
+  <si>
+    <t>data/derived/GBR3/GBR3_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/GBR3/GBR3_regions.RDS</t>
   </si>
 </sst>
 </file>
@@ -511,19 +520,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC09EBF-A19C-5D4E-8812-2D348421568B}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -557,7 +566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -574,7 +583,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -591,7 +600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -608,7 +617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -625,7 +634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -642,7 +651,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -659,7 +668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -676,7 +685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -693,7 +702,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -710,7 +719,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -727,7 +736,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -744,7 +753,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -761,7 +770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -778,7 +787,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -792,6 +801,40 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
         <v>16</v>
       </c>
     </row>
@@ -808,9 +851,9 @@
       <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -827,7 +870,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -844,7 +887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -861,7 +904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
🧹 raw seroval and paths for deriv
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC09CF62-D348-445E-BA7D-C2529EDE7F25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A515C6-764E-0D45-A29E-544343FA8DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>NYC_NY_1</t>
   </si>
   <si>
-    <t>data/derived/USA/NYC_NY_1_agebands.RDS</t>
-  </si>
-  <si>
     <t>data/derived/CHE/CHE_region.RDS</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>data/derived/CHE2/CHE2_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/USA/NYC_NY_1agebands.RDS</t>
   </si>
 </sst>
 </file>
@@ -529,16 +529,16 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="32.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,9 +555,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -572,9 +572,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -589,7 +589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -606,7 +606,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -623,7 +623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -640,7 +640,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -657,7 +657,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -674,7 +674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -682,7 +682,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -691,7 +691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -708,7 +708,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -725,7 +725,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -733,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -742,67 +742,67 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>35</v>
       </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
         <v>38</v>
       </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
       <c r="D16" t="s">
         <v>17</v>
       </c>
@@ -810,16 +810,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
         <v>41</v>
       </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>42</v>
-      </c>
       <c r="D17" t="s">
         <v>17</v>
       </c>
@@ -827,32 +827,32 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>43</v>
       </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
         <v>44</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -874,9 +874,9 @@
       <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -893,7 +893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -910,15 +910,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -927,15 +927,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
distinguish che1 v 2
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A515C6-764E-0D45-A29E-544343FA8DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7463DA7-3630-CB4E-8BE6-569C3E8582EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>CHE1</t>
   </si>
   <si>
-    <t>data/derived/CHE/CHE_agebands.RDS</t>
-  </si>
-  <si>
     <t>SWE1</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>NYC_NY_1</t>
   </si>
   <si>
-    <t>data/derived/CHE/CHE_region.RDS</t>
-  </si>
-  <si>
     <t>GBR2</t>
   </si>
   <si>
@@ -164,6 +158,12 @@
   </si>
   <si>
     <t>data/derived/USA/NYC_NY_1agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/CHE/CHE1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/CHE/CHE1_region.RDS</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,7 +557,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -665,7 +665,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -682,7 +682,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -693,47 +693,47 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -744,13 +744,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
@@ -761,13 +761,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -778,13 +778,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -795,13 +795,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -812,13 +812,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -829,13 +829,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
@@ -846,13 +846,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -878,13 +878,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>17</v>
@@ -895,13 +895,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -912,36 +912,36 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update new derived data
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7463DA7-3630-CB4E-8BE6-569C3E8582EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6B8189-D40A-FE48-B1E2-63D915819C74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
@@ -160,10 +160,10 @@
     <t>data/derived/USA/NYC_NY_1agebands.RDS</t>
   </si>
   <si>
-    <t>data/derived/CHE/CHE1_agebands.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/CHE/CHE1_region.RDS</t>
+    <t>data/derived/CHE1/CHE1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/CHE1/CHE1_region.RDS</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Add deaths to denominator of IFR calculation. Correct CHE filename.
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7463DA7-3630-CB4E-8BE6-569C3E8582EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E70FC5-33CC-4591-9CF6-FD028EA52A4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,10 +160,10 @@
     <t>data/derived/USA/NYC_NY_1agebands.RDS</t>
   </si>
   <si>
-    <t>data/derived/CHE/CHE1_agebands.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/CHE/CHE1_region.RDS</t>
+    <t>data/derived/CHE1/CHE1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/CHE1/CHE1_region.RDS</t>
   </si>
 </sst>
 </file>
@@ -532,13 +532,13 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -572,7 +572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -589,7 +589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -606,7 +606,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -623,7 +623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -640,7 +640,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -657,7 +657,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -674,7 +674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -691,7 +691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -708,7 +708,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -725,7 +725,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -742,7 +742,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -759,7 +759,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -776,7 +776,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -793,7 +793,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -810,7 +810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -827,7 +827,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -844,7 +844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -874,9 +874,9 @@
       <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -893,7 +893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -910,7 +910,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -927,7 +927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Correct Kenya, add graphs.
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E70FC5-33CC-4591-9CF6-FD028EA52A4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C3C89B-4A54-4F9A-AE82-AEB2AACDF127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="48">
   <si>
     <t>study_id</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>data/derived/CHE1/CHE1_region.RDS</t>
+  </si>
+  <si>
+    <t>KEN1</t>
+  </si>
+  <si>
+    <t>data/derived/KEN/KEN_agebands.RDS</t>
   </si>
 </sst>
 </file>
@@ -526,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC09EBF-A19C-5D4E-8812-2D348421568B}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -858,6 +864,23 @@
         <v>4</v>
       </c>
       <c r="E19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update derived data map and run process data and descriptive plots
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6B8189-D40A-FE48-B1E2-63D915819C74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C939D4F6-0D19-4F77-84EA-83749F6E3864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
   <si>
     <t>study_id</t>
   </si>
@@ -43,30 +43,12 @@
     <t>stratified</t>
   </si>
   <si>
-    <t>data/derived/ESP/ESP_agebands.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/ESP/ESP_regions.RDS</t>
-  </si>
-  <si>
     <t>relpath</t>
   </si>
   <si>
-    <t>data/derived/NLD/NLD_regions.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/NLD/NLD_agebands.RDS</t>
-  </si>
-  <si>
     <t>NLD1</t>
   </si>
   <si>
-    <t>data/derived/DNK/DNK_regions.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/DNK/DNK_agebands.RDS</t>
-  </si>
-  <si>
     <t>DNK1</t>
   </si>
   <si>
@@ -100,12 +82,6 @@
     <t>linelist</t>
   </si>
   <si>
-    <t>data/derived/BRA/BRA_regions.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/BRA/BRA_agebands.RDS</t>
-  </si>
-  <si>
     <t>NYC_NY_1</t>
   </si>
   <si>
@@ -121,24 +97,12 @@
     <t>ITA1</t>
   </si>
   <si>
-    <t>data/derived/ITA/ITA_regions.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/ITA/ITA_agebands.RDS</t>
-  </si>
-  <si>
     <t>CHN1</t>
   </si>
   <si>
     <t>LUX1</t>
   </si>
   <si>
-    <t>data/derived/CHN/CHN_agebands.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/LUX/LUX_agebands.RDS</t>
-  </si>
-  <si>
     <t>data/derived/UK/GBR2_regions.RDS</t>
   </si>
   <si>
@@ -164,6 +128,39 @@
   </si>
   <si>
     <t>data/derived/CHE1/CHE1_region.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/ESP1-2/ESP1-2_regions.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/ESP1-2/ESP1-2_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/NLD1/NLD1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/DNK1/DNK1_regions.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/DNK1/DNK1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/BRA1/BRA1_regions.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/BRA1/BRA1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/ITA1/ITA1_regions.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/ITA1/ITA1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/CHN1/CHN1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/LUX1/LUX1_agebands.RDS</t>
   </si>
 </sst>
 </file>
@@ -526,19 +523,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC09EBF-A19C-5D4E-8812-2D348421568B}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,319 +543,302 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
       <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
       <c r="E18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -874,74 +854,74 @@
       <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
care home data processing and plots
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C939D4F6-0D19-4F77-84EA-83749F6E3864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BF5538-1BFB-4101-BE3D-C870720E8D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="60">
   <si>
     <t>study_id</t>
   </si>
@@ -161,6 +161,51 @@
   </si>
   <si>
     <t>data/derived/LUX1/LUX1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>DNK1_nch</t>
+  </si>
+  <si>
+    <t>care_home_deaths</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>ESP1-2_nch</t>
+  </si>
+  <si>
+    <t>GBR3_nch</t>
+  </si>
+  <si>
+    <t>CHE1_nch</t>
+  </si>
+  <si>
+    <t>CHE2_nch</t>
+  </si>
+  <si>
+    <t>NYC_NY_1_nch</t>
+  </si>
+  <si>
+    <t>data/derived/DNK1/DNK1_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/ESP1-2/ESP1-2_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/GBR3/GBR3_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/CHE1/CHE1_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/CHE2/CHE2_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/USA/NYC_NY_1_agebands_noCH.RDS</t>
   </si>
 </sst>
 </file>
@@ -523,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC09EBF-A19C-5D4E-8812-2D348421568B}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -535,7 +580,7 @@
     <col min="4" max="5" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,8 +596,11 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -568,8 +616,11 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -585,8 +636,11 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -602,8 +656,11 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -619,8 +676,11 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -636,8 +696,11 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -653,8 +716,11 @@
       <c r="E7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -670,8 +736,11 @@
       <c r="E8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -687,8 +756,11 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -704,8 +776,11 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -721,8 +796,11 @@
       <c r="E11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -738,8 +816,11 @@
       <c r="E12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -755,8 +836,11 @@
       <c r="E13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -772,8 +856,11 @@
       <c r="E14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -789,8 +876,11 @@
       <c r="E15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -806,8 +896,11 @@
       <c r="E16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -823,8 +916,11 @@
       <c r="E17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -839,6 +935,129 @@
       </c>
       <c r="E18" t="s">
         <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix a few errors in descriptive plots
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BF5538-1BFB-4101-BE3D-C870720E8D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E4DD56-898F-4986-BB20-0E38FBA6A79D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="71">
   <si>
     <t>study_id</t>
   </si>
@@ -206,6 +206,39 @@
   </si>
   <si>
     <t>data/derived/USA/NYC_NY_1_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>China, Wuhan</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>England</t>
   </si>
 </sst>
 </file>
@@ -568,495 +601,567 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC09EBF-A19C-5D4E-8812-2D348421568B}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="32.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
       <c r="F7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
       <c r="F8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
       <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
         <v>40</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
       <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>41</v>
       </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
         <v>43</v>
       </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
         <v>44</v>
       </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
         <v>27</v>
       </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>28</v>
       </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>4</v>
       </c>
-      <c r="E18" t="s">
-        <v>10</v>
-      </c>
       <c r="F18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
         <v>54</v>
       </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
         <v>55</v>
       </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
         <v>56</v>
       </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
         <v>57</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>4</v>
       </c>
-      <c r="E22" t="s">
-        <v>10</v>
-      </c>
       <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
         <v>58</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>4</v>
       </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
       <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
         <v>59</v>
       </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update descriptive data and derived data
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BF5538-1BFB-4101-BE3D-C870720E8D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D101C102-3A08-DB47-9223-6285919DD29E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="57">
   <si>
     <t>study_id</t>
   </si>
@@ -40,9 +40,6 @@
     <t>region</t>
   </si>
   <si>
-    <t>stratified</t>
-  </si>
-  <si>
     <t>relpath</t>
   </si>
   <si>
@@ -52,12 +49,6 @@
     <t>DNK1</t>
   </si>
   <si>
-    <t>serology_type</t>
-  </si>
-  <si>
-    <t>death_type</t>
-  </si>
-  <si>
     <t>aggregate</t>
   </si>
   <si>
@@ -190,22 +181,22 @@
     <t>NYC_NY_1_nch</t>
   </si>
   <si>
-    <t>data/derived/DNK1/DNK1_agebands_noCH.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/ESP1-2/ESP1-2_agebands_noCH.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/GBR3/GBR3_agebands_noCH.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/CHE1/CHE1_agebands_noCH.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/CHE2/CHE2_agebands_noCH.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/USA/NYC_NY_1_agebands_noCH.RDS</t>
+    <t>data/derived/carehomes/DNK1_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/carehomes/ESP1-2_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/carehomes/GBR3_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/carehomes/CHE1_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/carehomes/CHE2_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/carehomes/NYC_NY_1_agebands_noCH.RDS</t>
   </si>
 </sst>
 </file>
@@ -568,19 +559,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC09EBF-A19C-5D4E-8812-2D348421568B}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="32.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,476 +578,332 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
       <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
         <v>45</v>
       </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
         <v>54</v>
       </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>49</v>
       </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
         <v>55</v>
       </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>50</v>
       </c>
-      <c r="B21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
         <v>56</v>
       </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>59</v>
-      </c>
       <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1073,74 +919,74 @@
       <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix non integer in care home data
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E4DD56-898F-4986-BB20-0E38FBA6A79D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318BAE66-B4B7-4026-95B4-8EAE9F1BF1DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
@@ -190,24 +190,6 @@
     <t>NYC_NY_1_nch</t>
   </si>
   <si>
-    <t>data/derived/DNK1/DNK1_agebands_noCH.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/ESP1-2/ESP1-2_agebands_noCH.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/GBR3/GBR3_agebands_noCH.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/CHE1/CHE1_agebands_noCH.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/CHE2/CHE2_agebands_noCH.RDS</t>
-  </si>
-  <si>
-    <t>data/derived/USA/NYC_NY_1_agebands_noCH.RDS</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
@@ -239,6 +221,24 @@
   </si>
   <si>
     <t>England</t>
+  </si>
+  <si>
+    <t>data/derived/carehomes/DNK1_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/carehomes/ESP1-2_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/carehomes/GBR3_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/carehomes/CHE1_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/carehomes/CHE2_agebands_noCH.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/carehomes/NYC_NY_1_agebands_noCH.RDS</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -641,7 +641,7 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -664,7 +664,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -687,7 +687,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -710,7 +710,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -733,7 +733,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -756,7 +756,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -779,7 +779,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -802,7 +802,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -825,7 +825,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -848,7 +848,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -871,7 +871,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -894,7 +894,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -917,7 +917,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -940,7 +940,7 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -963,7 +963,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -986,7 +986,7 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -1009,7 +1009,7 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -1032,13 +1032,13 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -1055,13 +1055,13 @@
         <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
@@ -1078,13 +1078,13 @@
         <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1101,13 +1101,13 @@
         <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
@@ -1124,13 +1124,13 @@
         <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
@@ -1147,13 +1147,13 @@
         <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
update fig1map and fig1
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBA1FAD-C211-0E42-BE39-1608045A69F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A1025D-DF35-5B44-962E-35EC5FAE7F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="460" windowWidth="25120" windowHeight="14660" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
+    <workbookView xWindow="4600" yWindow="4100" windowWidth="28940" windowHeight="16980" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="83">
   <si>
     <t>study_id</t>
   </si>
@@ -248,12 +248,6 @@
     <t>data/derived/KEN1/KEN1_agebands.RDS</t>
   </si>
   <si>
-    <t>BRA4</t>
-  </si>
-  <si>
-    <t>data/derived/BRA4/BRA4_regions.RDS</t>
-  </si>
-  <si>
     <t>BRA5</t>
   </si>
   <si>
@@ -266,21 +260,12 @@
     <t>data/derived/USA/LA_CA1_regions.RDS</t>
   </si>
   <si>
-    <t>SF_CA1</t>
-  </si>
-  <si>
-    <t>data/derived/USA/SF_CA1_regions.RDS</t>
-  </si>
-  <si>
     <t>Kenya</t>
   </si>
   <si>
     <t>USA, Los Angeles</t>
   </si>
   <si>
-    <t>USA, San Francisco</t>
-  </si>
-  <si>
     <t>USA, New York City</t>
   </si>
   <si>
@@ -291,9 +276,6 @@
   </si>
   <si>
     <t>Brazil, Rio Grande do Sul</t>
-  </si>
-  <si>
-    <t>Brazil, Rio de Janeiro</t>
   </si>
 </sst>
 </file>
@@ -676,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774DB1A2-37D9-E445-B702-DAB718EDD1BE}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -771,16 +753,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>47</v>
@@ -791,13 +773,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>47</v>
@@ -805,16 +787,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>47</v>
@@ -828,10 +810,10 @@
         <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>47</v>
@@ -839,16 +821,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>47</v>
@@ -856,16 +838,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>47</v>
@@ -873,16 +855,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>47</v>
@@ -890,16 +872,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>47</v>
@@ -907,16 +889,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>47</v>
@@ -930,10 +912,10 @@
         <v>64</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>47</v>
@@ -941,16 +923,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>47</v>
@@ -958,16 +940,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>47</v>
@@ -975,16 +957,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>47</v>
@@ -992,16 +974,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>47</v>
@@ -1009,67 +991,67 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>48</v>
@@ -1077,86 +1059,18 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="4" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update derived data map xlsx
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -1,33 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A1025D-DF35-5B44-962E-35EC5FAE7F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD58D81C-CEAE-421D-817D-E0A868FE4F7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4600" yWindow="4100" windowWidth="28940" windowHeight="16980" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="older" sheetId="1" r:id="rId2"/>
     <sheet name="oldest" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="76">
   <si>
     <t>study_id</t>
   </si>
@@ -248,34 +256,13 @@
     <t>data/derived/KEN1/KEN1_agebands.RDS</t>
   </si>
   <si>
-    <t>BRA5</t>
-  </si>
-  <si>
-    <t>data/derived/BRA5/BRA5_regions.RDS</t>
-  </si>
-  <si>
-    <t>LA_CA1</t>
-  </si>
-  <si>
-    <t>data/derived/USA/LA_CA1_regions.RDS</t>
-  </si>
-  <si>
     <t>Kenya</t>
   </si>
   <si>
-    <t>USA, Los Angeles</t>
-  </si>
-  <si>
-    <t>USA, New York City</t>
-  </si>
-  <si>
     <t>Switzerland, Geneva</t>
   </si>
   <si>
     <t>location</t>
-  </si>
-  <si>
-    <t>Brazil, Rio Grande do Sul</t>
   </si>
 </sst>
 </file>
@@ -658,20 +645,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774DB1A2-37D9-E445-B702-DAB718EDD1BE}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -683,7 +670,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -700,7 +687,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -717,7 +704,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -734,7 +721,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -742,21 +729,21 @@
         <v>57</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>2</v>
@@ -768,24 +755,24 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -793,284 +780,199 @@
         <v>59</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1087,13 +989,13 @@
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1018,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1139,7 +1041,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1162,7 +1064,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1185,7 +1087,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1208,7 +1110,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1231,7 +1133,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1254,7 +1156,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1277,7 +1179,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1300,7 +1202,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1323,7 +1225,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1346,7 +1248,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1369,7 +1271,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1392,7 +1294,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1415,7 +1317,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1438,7 +1340,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1461,7 +1363,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1484,7 +1386,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1507,7 +1409,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1530,7 +1432,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1553,7 +1455,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1576,7 +1478,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1599,7 +1501,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1622,7 +1524,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1661,9 +1563,9 @@
       <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1680,7 +1582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1697,7 +1599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1714,7 +1616,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Add, process, save data for age regional model
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD58D81C-CEAE-421D-817D-E0A868FE4F7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F4C982-FC0E-4D15-A478-4CCFCDEC52F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="80">
   <si>
     <t>study_id</t>
   </si>
@@ -263,6 +263,18 @@
   </si>
   <si>
     <t>location</t>
+  </si>
+  <si>
+    <t>NYS1</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>data/derived/USA/NYS1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>data/derived/USA/NYS1_regions.RDS</t>
   </si>
 </sst>
 </file>
@@ -645,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774DB1A2-37D9-E445-B702-DAB718EDD1BE}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -740,16 +752,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>47</v>
@@ -757,16 +769,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>47</v>
@@ -780,10 +792,10 @@
         <v>59</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>47</v>
@@ -791,16 +803,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>47</v>
@@ -808,16 +820,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>47</v>
@@ -825,16 +837,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>47</v>
@@ -842,16 +854,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>47</v>
@@ -859,16 +871,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>47</v>
@@ -876,16 +888,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>47</v>
@@ -893,16 +905,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>47</v>
@@ -910,69 +922,133 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>48</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update derived data map
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\GitHub\reestimate_covidIFR_analysis\data\derived\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F4C982-FC0E-4D15-A478-4CCFCDEC52F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A88797-2DEB-5D4E-BA68-11F0F9E3C80B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="4" r:id="rId1"/>
@@ -22,20 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="86">
   <si>
     <t>study_id</t>
   </si>
@@ -268,13 +260,31 @@
     <t>NYS1</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>data/derived/USA/NYS1_agebands.RDS</t>
   </si>
   <si>
     <t>data/derived/USA/NYS1_regions.RDS</t>
+  </si>
+  <si>
+    <t>Switzerland, Zurich</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>data/derived/SWE1/SWE1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>LA_CA1</t>
+  </si>
+  <si>
+    <t>USA, Los Angeles</t>
+  </si>
+  <si>
+    <t>data/derived/USA/LA_CA1_agebands.RDS</t>
+  </si>
+  <si>
+    <t>USA, New York State</t>
   </si>
 </sst>
 </file>
@@ -657,15 +667,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774DB1A2-37D9-E445-B702-DAB718EDD1BE}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -682,7 +692,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -699,7 +709,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -716,7 +726,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -733,7 +743,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -750,7 +760,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -767,7 +777,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -784,7 +794,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -801,7 +811,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -818,7 +828,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -835,7 +845,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -852,7 +862,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -869,7 +879,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -886,7 +896,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
@@ -903,7 +913,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -920,12 +930,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>2</v>
@@ -937,118 +947,156 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="E18" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1065,13 +1113,13 @@
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="32.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1142,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1117,7 +1165,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1140,7 +1188,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1163,7 +1211,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1186,7 +1234,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1209,7 +1257,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1232,7 +1280,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1255,7 +1303,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1278,7 +1326,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1301,7 +1349,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1324,7 +1372,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1347,7 +1395,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1370,7 +1418,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1393,7 +1441,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1416,7 +1464,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1439,7 +1487,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1462,7 +1510,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1485,7 +1533,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1508,7 +1556,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1531,7 +1579,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1554,7 +1602,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1577,7 +1625,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1600,7 +1648,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1639,9 +1687,9 @@
       <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1658,7 +1706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1675,7 +1723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1692,7 +1740,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
fixing large file issue
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB8E459-3E54-F74A-BCD8-B5251D02CEFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01A7D54-F4CD-E84A-9FCF-E6326D75024E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="86">
   <si>
     <t>study_id</t>
   </si>
@@ -667,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774DB1A2-37D9-E445-B702-DAB718EDD1BE}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A22" sqref="A22:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,91 +1033,6 @@
       </c>
       <c r="E21" s="4" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update results and analyses
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800DD592-08DE-1647-9284-90E02B277B75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F6CA5A-5256-D641-8CD7-57773307B41C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="90">
   <si>
     <t>study_id</t>
   </si>
@@ -286,6 +286,18 @@
   </si>
   <si>
     <t>Switzerland, Zurich</t>
+  </si>
+  <si>
+    <t>Wuhan, China</t>
+  </si>
+  <si>
+    <t>Geneva, Switzerland</t>
+  </si>
+  <si>
+    <t>Zurich, Switzerland</t>
+  </si>
+  <si>
+    <t>New York State, USA</t>
   </si>
 </sst>
 </file>
@@ -668,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548F9569-A157-DA46-8212-BB80E60294E4}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,7 +798,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
@@ -871,7 +883,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>2</v>
@@ -922,7 +934,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>2</v>
@@ -953,16 +965,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>47</v>
@@ -973,32 +985,15 @@
         <v>76</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="4" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
exclude wuhan w/ updated preprint showing unclear serovalidation
</commit_message>
<xml_diff>
--- a/data/derived/derived_data_map.xlsx
+++ b/data/derived/derived_data_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbrazeau/Documents/GitHub/reestimate_covidIFR_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F6CA5A-5256-D641-8CD7-57773307B41C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA12E7FA-C380-5943-B061-CC50C6A2D14A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{0665B27F-7A9C-5446-9DE9-B018B28EA631}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="89">
   <si>
     <t>study_id</t>
   </si>
@@ -286,9 +286,6 @@
   </si>
   <si>
     <t>Switzerland, Zurich</t>
-  </si>
-  <si>
-    <t>Wuhan, China</t>
   </si>
   <si>
     <t>Geneva, Switzerland</t>
@@ -680,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548F9569-A157-DA46-8212-BB80E60294E4}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,7 +795,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
@@ -880,16 +877,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>47</v>
@@ -903,10 +900,10 @@
         <v>64</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>47</v>
@@ -914,16 +911,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>47</v>
@@ -931,16 +928,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>47</v>
@@ -948,16 +945,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>47</v>
@@ -968,32 +965,15 @@
         <v>76</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="4" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>